<commit_message>
We added a new LS coolingFinQuadLiveScript.mlx
</commit_message>
<xml_diff>
--- a/tempCoolingFinTriang.xlsx
+++ b/tempCoolingFinTriang.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="5">
   <si>
     <t>NumNod</t>
   </si>
@@ -48,7 +48,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -72,11 +72,47 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -94,6 +130,42 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -114,19 +186,19 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="51" t="s">
         <v>4</v>
       </c>
     </row>
@@ -141,10 +213,10 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>40.796708844770507</v>
+        <v>40.796708844770642</v>
       </c>
       <c r="E2">
-        <v>-0.68190483243935462</v>
+        <v>-0.68190483243935329</v>
       </c>
     </row>
     <row r="3">
@@ -158,10 +230,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>43.982004676407698</v>
+        <v>43.98200467640779</v>
       </c>
       <c r="E3">
-        <v>-0.30486195691625795</v>
+        <v>-0.30486195691626072</v>
       </c>
     </row>
     <row r="4">
@@ -175,10 +247,10 @@
         <v>1.7999999499999999</v>
       </c>
       <c r="D4">
-        <v>41.474636583164774</v>
+        <v>41.474636583164902</v>
       </c>
       <c r="E4">
-        <v>-0.58455768423846954</v>
+        <v>-0.58455768423846877</v>
       </c>
     </row>
     <row r="5">
@@ -192,10 +264,10 @@
         <v>1.60000002</v>
       </c>
       <c r="D5">
-        <v>42.039373275183308</v>
+        <v>42.039373275183436</v>
       </c>
       <c r="E5">
-        <v>-0.59024740094598349</v>
+        <v>-0.59024740094598016</v>
       </c>
     </row>
     <row r="6">
@@ -209,10 +281,10 @@
         <v>1.39999998</v>
       </c>
       <c r="D6">
-        <v>42.516337158357558</v>
+        <v>42.516337158357679</v>
       </c>
       <c r="E6">
-        <v>-0.59503675862399685</v>
+        <v>-0.59503675862399419</v>
       </c>
     </row>
     <row r="7">
@@ -226,10 +298,10 @@
         <v>1.2000000500000001</v>
       </c>
       <c r="D7">
-        <v>42.917360283884435</v>
+        <v>42.917360283884548</v>
       </c>
       <c r="E7">
-        <v>-0.59905824722856038</v>
+        <v>-0.59905824722855527</v>
       </c>
     </row>
     <row r="8">
@@ -243,10 +315,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>43.249187795134461</v>
+        <v>43.249187795134567</v>
       </c>
       <c r="E8">
-        <v>-0.60238384990058469</v>
+        <v>-0.60238384990058691</v>
       </c>
     </row>
     <row r="9">
@@ -260,10 +332,10 @@
         <v>0.80000001200000004</v>
       </c>
       <c r="D9">
-        <v>43.516164232867737</v>
+        <v>43.516164232867837</v>
       </c>
       <c r="E9">
-        <v>-0.60505845726963725</v>
+        <v>-0.60505845726964935</v>
       </c>
     </row>
     <row r="10">
@@ -277,10 +349,10 @@
         <v>0.60000002399999997</v>
       </c>
       <c r="D10">
-        <v>43.721251417284435</v>
+        <v>43.721251417284549</v>
       </c>
       <c r="E10">
-        <v>-0.60711275665289344</v>
+        <v>-0.60711275665287978</v>
       </c>
     </row>
     <row r="11">
@@ -294,10 +366,10 @@
         <v>0.40000000600000002</v>
       </c>
       <c r="D11">
-        <v>43.866478599443113</v>
+        <v>43.866478599443212</v>
       </c>
       <c r="E11">
-        <v>-0.60856724504901794</v>
+        <v>-0.60856724504901649</v>
       </c>
     </row>
     <row r="12">
@@ -311,10 +383,10 @@
         <v>0.20000000300000001</v>
       </c>
       <c r="D12">
-        <v>43.953162053182766</v>
+        <v>43.953162053182858</v>
       </c>
       <c r="E12">
-        <v>-0.60943522828915397</v>
+        <v>-0.60943522828915775</v>
       </c>
     </row>
     <row r="13">
@@ -345,10 +417,10 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>45.551381035561306</v>
+        <v>45.551381035561398</v>
       </c>
       <c r="E14">
-        <v>-1.6488645149673141e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -362,10 +434,10 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>47.212245086635896</v>
+        <v>47.212245086635974</v>
       </c>
       <c r="E15">
-        <v>4.4047439975569324e-15</v>
+        <v>-8.7707618945387367e-15</v>
       </c>
     </row>
     <row r="16">
@@ -379,10 +451,10 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>48.964993432467082</v>
+        <v>48.964993432467168</v>
       </c>
       <c r="E16">
-        <v>6.3390923266830038e-15</v>
+        <v>-2.6645352591003757e-15</v>
       </c>
     </row>
     <row r="17">
@@ -396,10 +468,10 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>50.809017213154227</v>
+        <v>50.809017213154327</v>
       </c>
       <c r="E17">
-        <v>-9.6655850897449276e-15</v>
+        <v>-1.354472090042691e-14</v>
       </c>
     </row>
     <row r="18">
@@ -413,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>52.742867421030461</v>
+        <v>52.74286742103056</v>
       </c>
       <c r="E18">
-        <v>8.8303089402630251e-15</v>
+        <v>1.6764367671839864e-14</v>
       </c>
     </row>
     <row r="19">
@@ -430,10 +502,10 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>54.764429391583036</v>
+        <v>54.764429391583114</v>
       </c>
       <c r="E19">
-        <v>-7.0643409358060886e-15</v>
+        <v>-5.8841820305133297e-15</v>
       </c>
     </row>
     <row r="20">
@@ -447,10 +519,10 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>56.871061885491663</v>
+        <v>56.871061885491734</v>
       </c>
       <c r="E20">
-        <v>1.6566670797914124e-14</v>
+        <v>1.6764367671839864e-14</v>
       </c>
     </row>
     <row r="21">
@@ -464,10 +536,10 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>59.059686000686341</v>
+        <v>59.059686000686412</v>
       </c>
       <c r="E21">
-        <v>-8.3049379426292915e-15</v>
+        <v>-1.2545520178264269e-14</v>
       </c>
     </row>
     <row r="22">
@@ -481,10 +553,10 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>61.326826051997358</v>
+        <v>61.326826051997422</v>
       </c>
       <c r="E22">
-        <v>-5.9853086782176016e-15</v>
+        <v>-9.9920072216264089e-16</v>
       </c>
     </row>
     <row r="23">
@@ -498,10 +570,10 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>63.668612224966566</v>
+        <v>63.668612224966608</v>
       </c>
       <c r="E23">
-        <v>8.7263091654905821e-15</v>
+        <v>3.9968028886505635e-15</v>
       </c>
     </row>
     <row r="24">
@@ -515,10 +587,10 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>66.080756967248561</v>
+        <v>66.08075696724859</v>
       </c>
       <c r="E24">
-        <v>-5.4255683391674881e-15</v>
+        <v>-6.106226635438361e-15</v>
       </c>
     </row>
     <row r="25">
@@ -532,10 +604,10 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>68.558516700128237</v>
+        <v>68.558516700128251</v>
       </c>
       <c r="E25">
-        <v>-3.6243736401920043e-15</v>
+        <v>-1.5210055437364645e-14</v>
       </c>
     </row>
     <row r="26">
@@ -552,7 +624,7 @@
         <v>71.096649302252416</v>
       </c>
       <c r="E26">
-        <v>8.5638948581595602e-15</v>
+        <v>-5.6621374255882984e-15</v>
       </c>
     </row>
     <row r="27">
@@ -566,10 +638,10 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>73.689376681437579</v>
+        <v>73.689376681437594</v>
       </c>
       <c r="E27">
-        <v>-6.1230283229935922e-15</v>
+        <v>-1.5432100042289676e-14</v>
       </c>
     </row>
     <row r="28">
@@ -583,10 +655,10 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>76.330360730833775</v>
+        <v>76.330360730833789</v>
       </c>
       <c r="E28">
-        <v>9.7517218769475346e-15</v>
+        <v>1.6209256159527285e-14</v>
       </c>
     </row>
     <row r="29">
@@ -600,10 +672,10 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>79.012699898643092</v>
+        <v>79.012699898643106</v>
       </c>
       <c r="E29">
-        <v>-1.0156894717769294e-14</v>
+        <v>-1.9206858326015208e-14</v>
       </c>
     </row>
     <row r="30">
@@ -617,10 +689,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>81.728952195108661</v>
+        <v>81.728952195108675</v>
       </c>
       <c r="E30">
-        <v>1.5446973247793569e-15</v>
+        <v>6.5503158452884236e-15</v>
       </c>
     </row>
     <row r="31">
@@ -634,10 +706,10 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>84.471188494847425</v>
+        <v>84.471188494847439</v>
       </c>
       <c r="E31">
-        <v>-7.9350812411106208e-15</v>
+        <v>4.8849813083506888e-15</v>
       </c>
     </row>
     <row r="32">
@@ -654,7 +726,7 @@
         <v>87.231077410602012</v>
       </c>
       <c r="E32">
-        <v>2.0739885192521536e-14</v>
+        <v>1.6764367671839864e-14</v>
       </c>
     </row>
     <row r="33">
@@ -671,7 +743,7 @@
         <v>90</v>
       </c>
       <c r="E33">
-        <v>1.4852973901923798</v>
+        <v>1.4852973901923789</v>
       </c>
     </row>
     <row r="34">
@@ -688,7 +760,7 @@
         <v>90</v>
       </c>
       <c r="E34">
-        <v>2.2246665352685477</v>
+        <v>2.2246665352685584</v>
       </c>
     </row>
     <row r="35">
@@ -705,7 +777,7 @@
         <v>90</v>
       </c>
       <c r="E35">
-        <v>2.2525445289968529</v>
+        <v>2.2525445289968955</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +794,7 @@
         <v>90</v>
       </c>
       <c r="E36">
-        <v>2.3002488353543202</v>
+        <v>2.3002488353543278</v>
       </c>
     </row>
     <row r="37">
@@ -739,7 +811,7 @@
         <v>90</v>
       </c>
       <c r="E37">
-        <v>2.3703480717217635</v>
+        <v>2.3703480717217644</v>
       </c>
     </row>
     <row r="38">
@@ -756,7 +828,7 @@
         <v>90</v>
       </c>
       <c r="E38">
-        <v>2.4673031254134421</v>
+        <v>2.4673031254134656</v>
       </c>
     </row>
     <row r="39">
@@ -773,7 +845,7 @@
         <v>90</v>
       </c>
       <c r="E39">
-        <v>2.5989423062572867</v>
+        <v>2.5989423062572996</v>
       </c>
     </row>
     <row r="40">
@@ -790,7 +862,7 @@
         <v>90</v>
       </c>
       <c r="E40">
-        <v>2.7799595641862749</v>
+        <v>2.7799595641862851</v>
       </c>
     </row>
     <row r="41">
@@ -807,7 +879,7 @@
         <v>90</v>
       </c>
       <c r="E41">
-        <v>3.0418182110238932</v>
+        <v>3.0418182110238945</v>
       </c>
     </row>
     <row r="42">
@@ -824,7 +896,7 @@
         <v>90</v>
       </c>
       <c r="E42">
-        <v>3.4707226225172891</v>
+        <v>3.4707226225173002</v>
       </c>
     </row>
     <row r="43">
@@ -841,7 +913,7 @@
         <v>85.049012000017413</v>
       </c>
       <c r="E43">
-        <v>-1.3757603642656735</v>
+        <v>-1.3757603642656768</v>
       </c>
     </row>
     <row r="44">
@@ -858,7 +930,7 @@
         <v>80.937419042810234</v>
       </c>
       <c r="E44">
-        <v>-1.3196163354482209</v>
+        <v>-1.3196163354482202</v>
       </c>
     </row>
     <row r="45">
@@ -872,10 +944,10 @@
         <v>3.7000000499999999</v>
       </c>
       <c r="D45">
-        <v>77.313134235249152</v>
+        <v>77.313134235249166</v>
       </c>
       <c r="E45">
-        <v>-1.2704715650821243</v>
+        <v>-1.2704715650821079</v>
       </c>
     </row>
     <row r="46">
@@ -889,10 +961,10 @@
         <v>3.5999998999999998</v>
       </c>
       <c r="D46">
-        <v>74.01957829780622</v>
+        <v>74.019578297806234</v>
       </c>
       <c r="E46">
-        <v>-1.2259463633869543</v>
+        <v>-1.2259463633869636</v>
       </c>
     </row>
     <row r="47">
@@ -906,10 +978,10 @@
         <v>3.5</v>
       </c>
       <c r="D47">
-        <v>70.974591526975033</v>
+        <v>70.974591526975061</v>
       </c>
       <c r="E47">
-        <v>-1.1848407920635933</v>
+        <v>-1.1848407920635857</v>
       </c>
     </row>
     <row r="48">
@@ -923,10 +995,10 @@
         <v>3.4000001000000002</v>
       </c>
       <c r="D48">
-        <v>68.128716192003949</v>
+        <v>68.128716192003978</v>
       </c>
       <c r="E48">
-        <v>-1.1464537928123457</v>
+        <v>-1.1464537928123413</v>
       </c>
     </row>
     <row r="49">
@@ -940,10 +1012,10 @@
         <v>3.2999999500000001</v>
       </c>
       <c r="D49">
-        <v>65.449226464594631</v>
+        <v>65.449226464594659</v>
       </c>
       <c r="E49">
-        <v>-1.1103285852831313</v>
+        <v>-1.1103285852831277</v>
       </c>
     </row>
     <row r="50">
@@ -957,10 +1029,10 @@
         <v>3.2000000499999999</v>
       </c>
       <c r="D50">
-        <v>62.913181103250459</v>
+        <v>62.913181103250501</v>
       </c>
       <c r="E50">
-        <v>-1.0761487857682666</v>
+        <v>-1.076148785768261</v>
       </c>
     </row>
     <row r="51">
@@ -974,10 +1046,10 @@
         <v>3.0999998999999998</v>
       </c>
       <c r="D51">
-        <v>60.503983921795715</v>
+        <v>60.503983921795758</v>
       </c>
       <c r="E51">
-        <v>-1.0436866945765992</v>
+        <v>-1.0436866945766141</v>
       </c>
     </row>
     <row r="52">
@@ -991,10 +1063,10 @@
         <v>3</v>
       </c>
       <c r="D52">
-        <v>58.209475239973216</v>
+        <v>58.209475239973273</v>
       </c>
       <c r="E52">
-        <v>-1.0127758964746076</v>
+        <v>-1.0127758964746008</v>
       </c>
     </row>
     <row r="53">
@@ -1008,10 +1080,10 @@
         <v>2.9000001000000002</v>
       </c>
       <c r="D53">
-        <v>56.020807599409132</v>
+        <v>56.020807599409181</v>
       </c>
       <c r="E53">
-        <v>-0.98329621326487682</v>
+        <v>-0.98329621326488237</v>
       </c>
     </row>
     <row r="54">
@@ -1025,10 +1097,10 @@
         <v>2.7999999500000001</v>
       </c>
       <c r="D54">
-        <v>53.931734829749409</v>
+        <v>53.931734829749473</v>
       </c>
       <c r="E54">
-        <v>-0.95516206129004066</v>
+        <v>-0.95516206129003578</v>
       </c>
     </row>
     <row r="55">
@@ -1042,10 +1114,10 @@
         <v>2.7000000499999999</v>
       </c>
       <c r="D55">
-        <v>51.938178463168512</v>
+        <v>51.938178463168576</v>
       </c>
       <c r="E55">
-        <v>-0.92831816659511313</v>
+        <v>-0.9283181665951119</v>
       </c>
     </row>
     <row r="56">
@@ -1059,10 +1131,10 @@
         <v>2.5999998999999998</v>
       </c>
       <c r="D56">
-        <v>50.037991838855874</v>
+        <v>50.037991838855945</v>
       </c>
       <c r="E56">
-        <v>-0.90273547894682638</v>
+        <v>-0.90273547894682693</v>
       </c>
     </row>
     <row r="57">
@@ -1076,10 +1148,10 @@
         <v>2.5</v>
       </c>
       <c r="D57">
-        <v>48.230887782929202</v>
+        <v>48.23088778292928</v>
       </c>
       <c r="E57">
-        <v>-0.87841031742884612</v>
+        <v>-0.87841031742884823</v>
       </c>
     </row>
     <row r="58">
@@ -1093,10 +1165,10 @@
         <v>2.4000001000000002</v>
       </c>
       <c r="D58">
-        <v>46.518593314250673</v>
+        <v>46.518593314250758</v>
       </c>
       <c r="E58">
-        <v>-0.85536749817624169</v>
+        <v>-0.85536749817624269</v>
       </c>
     </row>
     <row r="59">
@@ -1110,10 +1182,10 @@
         <v>2.2999999500000001</v>
       </c>
       <c r="D59">
-        <v>44.905342802999442</v>
+        <v>44.905342802999542</v>
       </c>
       <c r="E59">
-        <v>-0.8336664835027795</v>
+        <v>-0.83366648350277828</v>
       </c>
     </row>
     <row r="60">
@@ -1127,10 +1199,10 @@
         <v>2.2000000499999999</v>
       </c>
       <c r="D60">
-        <v>43.399173118406416</v>
+        <v>43.39917311840653</v>
       </c>
       <c r="E60">
-        <v>-0.81342428142267043</v>
+        <v>-0.81342428142266598</v>
       </c>
     </row>
     <row r="61">
@@ -1144,10 +1216,10 @@
         <v>2.0999998999999998</v>
       </c>
       <c r="D61">
-        <v>42.015785569424928</v>
+        <v>42.015785569425056</v>
       </c>
       <c r="E61">
-        <v>-0.79489304089689117</v>
+        <v>-0.79489304089689838</v>
       </c>
     </row>
     <row r="62">
@@ -1164,7 +1236,7 @@
         <v>87.220388338455706</v>
       </c>
       <c r="E62">
-        <v>-1.8889271456403732e-14</v>
+        <v>4.8849813083506888e-15</v>
       </c>
     </row>
     <row r="63">
@@ -1181,7 +1253,7 @@
         <v>84.451058711571164</v>
       </c>
       <c r="E63">
-        <v>-7.3225835847077713e-15</v>
+        <v>1.2434497875801753e-14</v>
       </c>
     </row>
     <row r="64">
@@ -1198,7 +1270,7 @@
         <v>81.700716666313795</v>
       </c>
       <c r="E64">
-        <v>-8.2416170331504822e-15</v>
+        <v>-1.7763568394002505e-14</v>
       </c>
     </row>
     <row r="65">
@@ -1215,7 +1287,7 @@
         <v>78.977722337632002</v>
       </c>
       <c r="E65">
-        <v>2.1761028869333122e-14</v>
+        <v>1.5099033134902129e-14</v>
       </c>
     </row>
     <row r="66">
@@ -1229,10 +1301,10 @@
         <v>0.34999999399999998</v>
       </c>
       <c r="D66">
-        <v>76.289980703280079</v>
+        <v>76.289980703280094</v>
       </c>
       <c r="E66">
-        <v>4.8663016992380873e-15</v>
+        <v>7.5495165674510645e-15</v>
       </c>
     </row>
     <row r="67">
@@ -1246,10 +1318,10 @@
         <v>0.34000000400000002</v>
       </c>
       <c r="D67">
-        <v>73.644865108816802</v>
+        <v>73.64486510881683</v>
       </c>
       <c r="E67">
-        <v>1.1999406468870273e-15</v>
+        <v>3.0198066269804258e-14</v>
       </c>
     </row>
     <row r="68">
@@ -1263,10 +1335,10 @@
         <v>0.33000001299999998</v>
       </c>
       <c r="D68">
-        <v>71.049174938528466</v>
+        <v>71.049174938528481</v>
       </c>
       <c r="E68">
-        <v>8.2535350266726814e-15</v>
+        <v>-1.9984014443252818e-14</v>
       </c>
     </row>
     <row r="69">
@@ -1280,10 +1352,10 @@
         <v>0.31999999299999998</v>
       </c>
       <c r="D69">
-        <v>68.509124531371739</v>
+        <v>68.509124531371768</v>
       </c>
       <c r="E69">
-        <v>1.71627421170744e-14</v>
+        <v>4.241051954068098e-14</v>
       </c>
     </row>
     <row r="70">
@@ -1297,10 +1369,10 @@
         <v>0.310000002</v>
       </c>
       <c r="D70">
-        <v>66.030358160808404</v>
+        <v>66.030358160808433</v>
       </c>
       <c r="E70">
-        <v>2.2613802389083381e-14</v>
+        <v>3.0864200084579352e-14</v>
       </c>
     </row>
     <row r="71">
@@ -1314,10 +1386,10 @@
         <v>0.30000001199999998</v>
       </c>
       <c r="D71">
-        <v>63.6179843853267</v>
+        <v>63.617984385326736</v>
       </c>
       <c r="E71">
-        <v>-2.4745394075273074e-14</v>
+        <v>-4.3520742565306136e-14</v>
       </c>
     </row>
     <row r="72">
@@ -1331,10 +1403,10 @@
         <v>0.28999999199999998</v>
       </c>
       <c r="D72">
-        <v>61.276621882980244</v>
+        <v>61.276621882980308</v>
       </c>
       <c r="E72">
-        <v>-2.8628134769312839e-14</v>
+        <v>-1.9984014443252818e-15</v>
       </c>
     </row>
     <row r="73">
@@ -1348,10 +1420,10 @@
         <v>0.280000001</v>
       </c>
       <c r="D73">
-        <v>59.010448401499573</v>
+        <v>59.010448401499652</v>
       </c>
       <c r="E73">
-        <v>-2.0356603234806038e-15</v>
+        <v>8.2156503822261584e-15</v>
       </c>
     </row>
     <row r="74">
@@ -1365,10 +1437,10 @@
         <v>0.27000001099999998</v>
       </c>
       <c r="D74">
-        <v>56.823243649479927</v>
+        <v>56.823243649479998</v>
       </c>
       <c r="E74">
-        <v>-5.9843128868837484e-15</v>
+        <v>-2.2648549702353193e-14</v>
       </c>
     </row>
     <row r="75">
@@ -1382,10 +1454,10 @@
         <v>0.25999999000000001</v>
       </c>
       <c r="D75">
-        <v>54.718415472584205</v>
+        <v>54.718415472584283</v>
       </c>
       <c r="E75">
-        <v>4.5413621549547435e-15</v>
+        <v>4.4408920985006262e-15</v>
       </c>
     </row>
     <row r="76">
@@ -1399,10 +1471,10 @@
         <v>0.25</v>
       </c>
       <c r="D76">
-        <v>52.698997473892824</v>
+        <v>52.698997473892923</v>
       </c>
       <c r="E76">
-        <v>1.487215012338525e-14</v>
+        <v>2.3314683517128287e-14</v>
       </c>
     </row>
     <row r="77">
@@ -1416,10 +1488,10 @@
         <v>0.23999999499999999</v>
       </c>
       <c r="D77">
-        <v>50.767605354400025</v>
+        <v>50.767605354400132</v>
       </c>
       <c r="E77">
-        <v>-5.8071696712532399e-14</v>
+        <v>-3.3750779948604759e-14</v>
       </c>
     </row>
     <row r="78">
@@ -1433,10 +1505,10 @@
         <v>0.23000000400000001</v>
       </c>
       <c r="D78">
-        <v>48.926340547999501</v>
+        <v>48.926340547999594</v>
       </c>
       <c r="E78">
-        <v>-2.0899493371478082e-14</v>
+        <v>-2.6867397195928788e-14</v>
       </c>
     </row>
     <row r="79">
@@ -1450,10 +1522,10 @@
         <v>0.219999999</v>
       </c>
       <c r="D79">
-        <v>47.176637930562073</v>
+        <v>47.176637930562165</v>
       </c>
       <c r="E79">
-        <v>-3.5648311062839877e-14</v>
+        <v>-2.6867397195928788e-14</v>
       </c>
     </row>
     <row r="80">
@@ -1467,10 +1539,10 @@
         <v>0.209999993</v>
       </c>
       <c r="D80">
-        <v>45.519071788123028</v>
+        <v>45.519071788123128</v>
       </c>
       <c r="E80">
-        <v>-2.8164959042479062e-15</v>
+        <v>-3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="81">
@@ -1484,10 +1556,10 @@
         <v>0.77999997099999996</v>
       </c>
       <c r="D81">
-        <v>87.187815982093781</v>
+        <v>87.187815982093753</v>
       </c>
       <c r="E81">
-        <v>-3.6321576890300387e-14</v>
+        <v>-9.4146912488213275e-14</v>
       </c>
     </row>
     <row r="82">
@@ -1501,10 +1573,10 @@
         <v>0.75999998999999996</v>
       </c>
       <c r="D82">
-        <v>84.389812828071641</v>
+        <v>84.389812828071626</v>
       </c>
       <c r="E82">
-        <v>3.6984632848008007e-14</v>
+        <v>2.2204460492503131e-14</v>
       </c>
     </row>
     <row r="83">
@@ -1518,10 +1590,10 @@
         <v>0.74000001000000004</v>
       </c>
       <c r="D83">
-        <v>81.614943007465953</v>
+        <v>81.614943007465939</v>
       </c>
       <c r="E83">
-        <v>-2.4891057812543851e-14</v>
+        <v>-3.9523939676655573e-14</v>
       </c>
     </row>
     <row r="84">
@@ -1538,7 +1610,7 @@
         <v>78.87163476155439</v>
       </c>
       <c r="E84">
-        <v>7.8312260890746456e-15</v>
+        <v>1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="85">
@@ -1552,10 +1624,10 @@
         <v>0.69999998799999996</v>
       </c>
       <c r="D85">
-        <v>76.167696095328026</v>
+        <v>76.16769609532804</v>
       </c>
       <c r="E85">
-        <v>-2.390625840617806e-14</v>
+        <v>-1.2878587085651816e-14</v>
       </c>
     </row>
     <row r="86">
@@ -1569,10 +1641,10 @@
         <v>0.68000000699999996</v>
       </c>
       <c r="D86">
-        <v>73.510266618543525</v>
+        <v>73.51026661854354</v>
       </c>
       <c r="E86">
-        <v>-5.6112323830492009e-14</v>
+        <v>-9.6367358537463588e-14</v>
       </c>
     </row>
     <row r="87">
@@ -1586,10 +1658,10 @@
         <v>0.66000002599999996</v>
       </c>
       <c r="D87">
-        <v>70.905811901143963</v>
+        <v>70.905811901143991</v>
       </c>
       <c r="E87">
-        <v>-7.474580194622899e-14</v>
+        <v>-6.0840221749458578e-14</v>
       </c>
     </row>
     <row r="88">
@@ -1603,10 +1675,10 @@
         <v>0.63999998599999997</v>
       </c>
       <c r="D88">
-        <v>68.360151014335059</v>
+        <v>68.360151014335088</v>
       </c>
       <c r="E88">
-        <v>4.0515691617787195e-15</v>
+        <v>-7.9936057773011271e-15</v>
       </c>
     </row>
     <row r="89">
@@ -1620,10 +1692,10 @@
         <v>0.62000000499999997</v>
       </c>
       <c r="D89">
-        <v>65.878507665409288</v>
+        <v>65.878507665409316</v>
       </c>
       <c r="E89">
-        <v>3.3922648293222601e-14</v>
+        <v>3.9968028886505635e-14</v>
       </c>
     </row>
     <row r="90">
@@ -1637,10 +1709,10 @@
         <v>0.60000002399999997</v>
       </c>
       <c r="D90">
-        <v>63.465575808122246</v>
+        <v>63.465575808122281</v>
       </c>
       <c r="E90">
-        <v>-2.287490489378303e-14</v>
+        <v>-3.6859404417555197e-14</v>
       </c>
     </row>
     <row r="91">
@@ -1654,10 +1726,10 @@
         <v>0.579999983</v>
       </c>
       <c r="D91">
-        <v>61.125590262787412</v>
+        <v>61.125590262787455</v>
       </c>
       <c r="E91">
-        <v>5.6773077150799839e-14</v>
+        <v>2.2204460492503131e-14</v>
       </c>
     </row>
     <row r="92">
@@ -1671,10 +1743,10 @@
         <v>0.560000002</v>
       </c>
       <c r="D92">
-        <v>58.86239424169689</v>
+        <v>58.862394241696968</v>
       </c>
       <c r="E92">
-        <v>-2.5817137461152474e-15</v>
+        <v>2.5313084961453569e-14</v>
       </c>
     </row>
     <row r="93">
@@ -1688,10 +1760,10 @@
         <v>0.540000021</v>
       </c>
       <c r="D93">
-        <v>56.679495440416375</v>
+        <v>56.679495440416446</v>
       </c>
       <c r="E93">
-        <v>-3.4809438719693965e-14</v>
+        <v>-3.5527136788005009e-14</v>
       </c>
     </row>
     <row r="94">
@@ -1705,10 +1777,10 @@
         <v>0.519999981</v>
       </c>
       <c r="D94">
-        <v>54.580099706259148</v>
+        <v>54.580099706259226</v>
       </c>
       <c r="E94">
-        <v>1.3586676821444957e-14</v>
+        <v>2.6645352591003757e-14</v>
       </c>
     </row>
     <row r="95">
@@ -1722,10 +1794,10 @@
         <v>0.5</v>
       </c>
       <c r="D95">
-        <v>52.567109836551914</v>
+        <v>52.567109836551992</v>
       </c>
       <c r="E95">
-        <v>2.1339834403323214e-14</v>
+        <v>6.6613381477509392e-15</v>
       </c>
     </row>
     <row r="96">
@@ -1739,10 +1811,10 @@
         <v>0.47999998900000002</v>
       </c>
       <c r="D96">
-        <v>50.643074241349296</v>
+        <v>50.643074241349389</v>
       </c>
       <c r="E96">
-        <v>2.8453065735998741e-14</v>
+        <v>3.5527136788005009e-14</v>
       </c>
     </row>
     <row r="97">
@@ -1756,10 +1828,10 @@
         <v>0.46000000800000002</v>
       </c>
       <c r="D97">
-        <v>48.81006849305269</v>
+        <v>48.810068493052782</v>
       </c>
       <c r="E97">
-        <v>1.2236898435235569e-14</v>
+        <v>1.021405182655144e-14</v>
       </c>
     </row>
     <row r="98">
@@ -1773,10 +1845,10 @@
         <v>0.439999998</v>
       </c>
       <c r="D98">
-        <v>47.069502393352892</v>
+        <v>47.069502393352984</v>
       </c>
       <c r="E98">
-        <v>-3.0544861262785374e-14</v>
+        <v>-4.6185277824406512e-14</v>
       </c>
     </row>
     <row r="99">
@@ -1790,10 +1862,10 @@
         <v>0.41999998700000002</v>
       </c>
       <c r="D99">
-        <v>45.421867074931328</v>
+        <v>45.421867074931427</v>
       </c>
       <c r="E99">
-        <v>-3.2948814819323684e-14</v>
+        <v>-4.2632564145606011e-14</v>
       </c>
     </row>
     <row r="100">
@@ -1807,10 +1879,10 @@
         <v>1.1699999599999999</v>
       </c>
       <c r="D100">
-        <v>87.131872309950566</v>
+        <v>87.131872309950552</v>
       </c>
       <c r="E100">
-        <v>-1.2738799708187639e-13</v>
+        <v>-1.0658141036401503e-13</v>
       </c>
     </row>
     <row r="101">
@@ -1824,10 +1896,10 @@
         <v>1.13999999</v>
       </c>
       <c r="D101">
-        <v>84.284901504680008</v>
+        <v>84.284901504679979</v>
       </c>
       <c r="E101">
-        <v>1.9265014782919815e-14</v>
+        <v>-2.4868995751603507e-14</v>
       </c>
     </row>
     <row r="102">
@@ -1844,7 +1916,7 @@
         <v>81.468448109378841</v>
       </c>
       <c r="E102">
-        <v>-6.6152784082024095e-14</v>
+        <v>-6.3948846218409017e-14</v>
       </c>
     </row>
     <row r="103">
@@ -1858,10 +1930,10 @@
         <v>1.0800000400000001</v>
       </c>
       <c r="D103">
-        <v>78.690999840838614</v>
+        <v>78.690999840838629</v>
       </c>
       <c r="E103">
-        <v>-9.7494764914447457e-15</v>
+        <v>-7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="104">
@@ -1875,10 +1947,10 @@
         <v>1.0499999499999999</v>
       </c>
       <c r="D104">
-        <v>75.960116861938573</v>
+        <v>75.960116861938602</v>
       </c>
       <c r="E104">
-        <v>-2.0466714021084061e-14</v>
+        <v>-2.8421709430404007e-14</v>
       </c>
     </row>
     <row r="105">
@@ -1892,10 +1964,10 @@
         <v>1.0199999799999999</v>
       </c>
       <c r="D105">
-        <v>73.282450395585485</v>
+        <v>73.282450395585514</v>
       </c>
       <c r="E105">
-        <v>4.43485915533817e-14</v>
+        <v>4.2632564145606011e-14</v>
       </c>
     </row>
     <row r="106">
@@ -1909,10 +1981,10 @@
         <v>0.99000001000000004</v>
       </c>
       <c r="D106">
-        <v>70.663814367291081</v>
+        <v>70.66381436729111</v>
       </c>
       <c r="E106">
-        <v>-3.1678832828332885e-14</v>
+        <v>-3.5527136788005009e-14</v>
       </c>
     </row>
     <row r="107">
@@ -1926,10 +1998,10 @@
         <v>0.959999979</v>
       </c>
       <c r="D107">
-        <v>68.109287419202118</v>
+        <v>68.109287419202147</v>
       </c>
       <c r="E107">
-        <v>-2.9415196778246658e-14</v>
+        <v>-3.5527136788005009e-14</v>
       </c>
     </row>
     <row r="108">
@@ -1943,10 +2015,10 @@
         <v>0.93000000699999996</v>
       </c>
       <c r="D108">
-        <v>65.623328921636059</v>
+        <v>65.623328921636073</v>
       </c>
       <c r="E108">
-        <v>-1.6022477788355718e-16</v>
+        <v>-3.5527136788005009e-14</v>
       </c>
     </row>
     <row r="109">
@@ -1960,10 +2032,10 @@
         <v>0.89999997600000003</v>
       </c>
       <c r="D109">
-        <v>63.209896783193415</v>
+        <v>63.20989678319345</v>
       </c>
       <c r="E109">
-        <v>-6.0128940722109711e-15</v>
+        <v>-3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="110">
@@ -1977,10 +2049,10 @@
         <v>0.87000000499999997</v>
       </c>
       <c r="D110">
-        <v>60.872556850286578</v>
+        <v>60.872556850286621</v>
       </c>
       <c r="E110">
-        <v>-2.1607612371130426e-15</v>
+        <v>-1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="111">
@@ -1994,10 +2066,10 @@
         <v>0.83999997400000004</v>
       </c>
       <c r="D111">
-        <v>58.614579086115747</v>
+        <v>58.614579086115803</v>
       </c>
       <c r="E111">
-        <v>1.0117170021822711e-14</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="112">
@@ -2011,10 +2083,10 @@
         <v>0.810000002</v>
       </c>
       <c r="D112">
-        <v>56.439012129036769</v>
+        <v>56.439012129036826</v>
       </c>
       <c r="E112">
-        <v>2.6495032392910124e-15</v>
+        <v>-1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="113">
@@ -2028,10 +2100,10 @@
         <v>0.77999997099999996</v>
       </c>
       <c r="D113">
-        <v>54.348729406269534</v>
+        <v>54.348729406269605</v>
       </c>
       <c r="E113">
-        <v>2.2648416125597973e-14</v>
+        <v>1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="114">
@@ -2045,10 +2117,10 @@
         <v>0.75</v>
       </c>
       <c r="D114">
-        <v>52.346431046462747</v>
+        <v>52.346431046462826</v>
       </c>
       <c r="E114">
-        <v>6.4939009953384077e-14</v>
+        <v>6.3948846218409017e-14</v>
       </c>
     </row>
     <row r="115">
@@ -2062,10 +2134,10 @@
         <v>0.72000002900000004</v>
       </c>
       <c r="D115">
-        <v>50.434582617968935</v>
+        <v>50.434582617969021</v>
       </c>
       <c r="E115">
-        <v>-2.4685696341336717e-14</v>
+        <v>-1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="116">
@@ -2079,10 +2151,10 @@
         <v>0.689999998</v>
       </c>
       <c r="D116">
-        <v>48.615262251391691</v>
+        <v>48.615262251391776</v>
       </c>
       <c r="E116">
-        <v>-1.3163224106462493e-14</v>
+        <v>-4.6185277824406512e-14</v>
       </c>
     </row>
     <row r="117">
@@ -2096,10 +2168,10 @@
         <v>0.66000002599999996</v>
       </c>
       <c r="D117">
-        <v>46.889894955577034</v>
+        <v>46.889894955577141</v>
       </c>
       <c r="E117">
-        <v>4.2659965500521959e-15</v>
+        <v>2.1316282072803006e-14</v>
       </c>
     </row>
     <row r="118">
@@ -2113,10 +2185,10 @@
         <v>0.62999999500000003</v>
       </c>
       <c r="D118">
-        <v>45.258887414761148</v>
+        <v>45.258887414761254</v>
       </c>
       <c r="E118">
-        <v>-8.0792475583459939e-15</v>
+        <v>-7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="119">
@@ -2133,7 +2205,7 @@
         <v>87.049777361184624</v>
       </c>
       <c r="E119">
-        <v>2.39876082704615e-15</v>
+        <v>1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="120">
@@ -2150,7 +2222,7 @@
         <v>84.131612148231355</v>
       </c>
       <c r="E120">
-        <v>-3.8567671860482328e-14</v>
+        <v>-4.9737991503207013e-14</v>
       </c>
     </row>
     <row r="121">
@@ -2167,7 +2239,7 @@
         <v>81.255423751211367</v>
       </c>
       <c r="E121">
-        <v>1.5051009616079627e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -2181,10 +2253,10 @@
         <v>1.44000006</v>
       </c>
       <c r="D122">
-        <v>78.429635244455739</v>
+        <v>78.429635244455767</v>
       </c>
       <c r="E122">
-        <v>-5.1753908877143746e-15</v>
+        <v>-3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="123">
@@ -2198,10 +2270,10 @@
         <v>1.39999998</v>
       </c>
       <c r="D123">
-        <v>75.661236883147751</v>
+        <v>75.661236883147794</v>
       </c>
       <c r="E123">
-        <v>-2.3660845146009555e-14</v>
+        <v>1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="124">
@@ -2215,10 +2287,10 @@
         <v>1.36000001</v>
       </c>
       <c r="D124">
-        <v>72.955953860336791</v>
+        <v>72.955953860336834</v>
       </c>
       <c r="E124">
-        <v>3.0340305215358221e-14</v>
+        <v>6.3948846218409017e-14</v>
       </c>
     </row>
     <row r="125">
@@ -2232,10 +2304,10 @@
         <v>1.32000005</v>
       </c>
       <c r="D125">
-        <v>70.318465015855026</v>
+        <v>70.31846501585504</v>
       </c>
       <c r="E125">
-        <v>4.1657070838123483e-14</v>
+        <v>2.8421709430404007e-14</v>
       </c>
     </row>
     <row r="126">
@@ -2249,10 +2321,10 @@
         <v>1.27999997</v>
       </c>
       <c r="D126">
-        <v>67.752630437776318</v>
+        <v>67.752630437776347</v>
       </c>
       <c r="E126">
-        <v>1.6980707880755936e-14</v>
+        <v>1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="127">
@@ -2266,10 +2338,10 @@
         <v>1.2400000099999999</v>
       </c>
       <c r="D127">
-        <v>65.261704104600184</v>
+        <v>65.261704104600227</v>
       </c>
       <c r="E127">
-        <v>-2.0589045974093409e-15</v>
+        <v>2.1316282072803006e-14</v>
       </c>
     </row>
     <row r="128">
@@ -2283,10 +2355,10 @@
         <v>1.2000000500000001</v>
       </c>
       <c r="D128">
-        <v>62.848521562331392</v>
+        <v>62.848521562331428</v>
       </c>
       <c r="E128">
-        <v>2.115735019570514e-14</v>
+        <v>1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="129">
@@ -2300,10 +2372,10 @@
         <v>1.1599999700000001</v>
       </c>
       <c r="D129">
-        <v>60.515656027390499</v>
+        <v>60.515656027390541</v>
       </c>
       <c r="E129">
-        <v>5.2137067022668887e-15</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="130">
@@ -2317,10 +2389,10 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="D130">
-        <v>58.265543938714615</v>
+        <v>58.265543938714657</v>
       </c>
       <c r="E130">
-        <v>3.7469088700326936e-14</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="131">
@@ -2334,10 +2406,10 @@
         <v>1.0800000400000001</v>
       </c>
       <c r="D131">
-        <v>56.100581075520836</v>
+        <v>56.100581075520921</v>
       </c>
       <c r="E131">
-        <v>-2.6613758725021458e-14</v>
+        <v>1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="132">
@@ -2351,10 +2423,10 @@
         <v>1.0399999600000001</v>
       </c>
       <c r="D132">
-        <v>54.023181815755109</v>
+        <v>54.023181815755187</v>
       </c>
       <c r="E132">
-        <v>7.3776500838227405e-15</v>
+        <v>3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="133">
@@ -2368,10 +2440,10 @@
         <v>1</v>
       </c>
       <c r="D133">
-        <v>52.035789280208832</v>
+        <v>52.035789280208917</v>
       </c>
       <c r="E133">
-        <v>-1.5052478966446096e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -2385,10 +2457,10 @@
         <v>0.959999979</v>
       </c>
       <c r="D134">
-        <v>50.140809961218601</v>
+        <v>50.140809961218686</v>
       </c>
       <c r="E134">
-        <v>1.0207575082750082e-15</v>
+        <v>-1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="135">
@@ -2402,10 +2474,10 @@
         <v>0.920000017</v>
       </c>
       <c r="D135">
-        <v>48.340421786122839</v>
+        <v>48.340421786122931</v>
       </c>
       <c r="E135">
-        <v>5.2315906764997139e-15</v>
+        <v>1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="136">
@@ -2419,10 +2491,10 @@
         <v>0.87999999500000003</v>
       </c>
       <c r="D136">
-        <v>46.636203878699028</v>
+        <v>46.636203878699128</v>
       </c>
       <c r="E136">
-        <v>8.1465712809826895e-15</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="137">
@@ -2436,10 +2508,10 @@
         <v>0.83999997400000004</v>
       </c>
       <c r="D137">
-        <v>45.02857259129069</v>
+        <v>45.028572591290789</v>
       </c>
       <c r="E137">
-        <v>7.3959588044185983e-15</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="138">
@@ -2453,10 +2525,10 @@
         <v>1.9500000500000001</v>
       </c>
       <c r="D138">
-        <v>86.93677619684513</v>
+        <v>86.936776196845116</v>
       </c>
       <c r="E138">
-        <v>-1.3431190319352421e-15</v>
+        <v>-5.6843418860808015e-14</v>
       </c>
     </row>
     <row r="139">
@@ -2470,10 +2542,10 @@
         <v>1.89999998</v>
       </c>
       <c r="D139">
-        <v>83.922048605023676</v>
+        <v>83.92204860502369</v>
       </c>
       <c r="E139">
-        <v>-3.9364708284108501e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -2487,10 +2559,10 @@
         <v>1.85000002</v>
       </c>
       <c r="D140">
-        <v>80.966360847652439</v>
+        <v>80.966360847652453</v>
       </c>
       <c r="E140">
-        <v>4.2151314325706335e-14</v>
+        <v>6.5725203057809267e-14</v>
       </c>
     </row>
     <row r="141">
@@ -2504,10 +2576,10 @@
         <v>1.7999999499999999</v>
       </c>
       <c r="D141">
-        <v>78.077661341760631</v>
+        <v>78.077661341760646</v>
       </c>
       <c r="E141">
-        <v>-7.2804458978872792e-16</v>
+        <v>1.7763568394002505e-15</v>
       </c>
     </row>
     <row r="142">
@@ -2521,10 +2593,10 @@
         <v>1.75</v>
       </c>
       <c r="D142">
-        <v>75.261686819980483</v>
+        <v>75.261686819980497</v>
       </c>
       <c r="E142">
-        <v>1.5751531182414067e-14</v>
+        <v>-1.2434497875801753e-14</v>
       </c>
     </row>
     <row r="143">
@@ -2538,10 +2610,10 @@
         <v>1.7000000500000001</v>
       </c>
       <c r="D143">
-        <v>72.522453259559725</v>
+        <v>72.522453259559754</v>
       </c>
       <c r="E143">
-        <v>-1.5411288807220585e-14</v>
+        <v>-1.5099033134902129e-14</v>
       </c>
     </row>
     <row r="144">
@@ -2555,10 +2627,10 @@
         <v>1.64999998</v>
       </c>
       <c r="D144">
-        <v>69.862738124603624</v>
+        <v>69.862738124603652</v>
       </c>
       <c r="E144">
-        <v>2.9224357868938711e-14</v>
+        <v>3.2862601528904634e-14</v>
       </c>
     </row>
     <row r="145">
@@ -2572,10 +2644,10 @@
         <v>1.60000002</v>
       </c>
       <c r="D145">
-        <v>67.284497664081385</v>
+        <v>67.284497664081414</v>
       </c>
       <c r="E145">
-        <v>2.8719783141858885e-15</v>
+        <v>-7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="146">
@@ -2589,10 +2661,10 @@
         <v>1.5499999499999999</v>
       </c>
       <c r="D146">
-        <v>64.789204043600833</v>
+        <v>64.78920404360089</v>
       </c>
       <c r="E146">
-        <v>-2.8878237571478842e-14</v>
+        <v>8.8817841970012523e-15</v>
       </c>
     </row>
     <row r="147">
@@ -2606,10 +2678,10 @@
         <v>1.5</v>
       </c>
       <c r="D147">
-        <v>62.378102167754449</v>
+        <v>62.378102167754498</v>
       </c>
       <c r="E147">
-        <v>-4.3573475978789414e-14</v>
+        <v>-4.7073456244106637e-14</v>
       </c>
     </row>
     <row r="148">
@@ -2623,10 +2695,10 @@
         <v>1.4500000500000001</v>
       </c>
       <c r="D148">
-        <v>60.052404939794528</v>
+        <v>60.052404939794577</v>
       </c>
       <c r="E148">
-        <v>-6.9624375258077258e-15</v>
+        <v>-1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="149">
@@ -2640,10 +2712,10 @@
         <v>1.39999998</v>
       </c>
       <c r="D149">
-        <v>57.813436866663714</v>
+        <v>57.813436866663771</v>
       </c>
       <c r="E149">
-        <v>-1.7674498449412802e-14</v>
+        <v>-1.9539925233402755e-14</v>
       </c>
     </row>
     <row r="150">
@@ -2657,10 +2729,10 @@
         <v>1.35000002</v>
       </c>
       <c r="D150">
-        <v>55.662739071705225</v>
+        <v>55.662739071705296</v>
       </c>
       <c r="E150">
-        <v>2.7923106273958706e-14</v>
+        <v>2.6645352591003757e-14</v>
       </c>
     </row>
     <row r="151">
@@ -2674,10 +2746,10 @@
         <v>1.2999999499999999</v>
       </c>
       <c r="D151">
-        <v>53.602141753561419</v>
+        <v>53.602141753561504</v>
       </c>
       <c r="E151">
-        <v>1.8626441817889165e-14</v>
+        <v>2.3092638912203256e-14</v>
       </c>
     </row>
     <row r="152">
@@ -2691,10 +2763,10 @@
         <v>1.25</v>
       </c>
       <c r="D152">
-        <v>51.63378959106592</v>
+        <v>51.633789591066005</v>
       </c>
       <c r="E152">
-        <v>3.460158727892531e-14</v>
+        <v>2.1316282072803006e-14</v>
       </c>
     </row>
     <row r="153">
@@ -2708,10 +2780,10 @@
         <v>1.2000000500000001</v>
       </c>
       <c r="D153">
-        <v>49.760091991113732</v>
+        <v>49.760091991113832</v>
       </c>
       <c r="E153">
-        <v>1.5361295694254638e-14</v>
+        <v>2.2204460492503131e-14</v>
       </c>
     </row>
     <row r="154">
@@ -2725,10 +2797,10 @@
         <v>1.14999998</v>
       </c>
       <c r="D154">
-        <v>47.983516203780347</v>
+        <v>47.983516203780454</v>
       </c>
       <c r="E154">
-        <v>-2.2063533392433995e-14</v>
+        <v>1.7763568394002505e-15</v>
       </c>
     </row>
     <row r="155">
@@ -2742,10 +2814,10 @@
         <v>1.10000002</v>
       </c>
       <c r="D155">
-        <v>46.306097562700693</v>
+        <v>46.306097562700792</v>
       </c>
       <c r="E155">
-        <v>3.7423252620417823e-14</v>
+        <v>3.3750779948604759e-14</v>
       </c>
     </row>
     <row r="156">
@@ -2759,10 +2831,10 @@
         <v>1.0499999499999999</v>
       </c>
       <c r="D156">
-        <v>44.728558225311822</v>
+        <v>44.728558225311929</v>
       </c>
       <c r="E156">
-        <v>6.1942383365996377e-16</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="157">
@@ -2776,10 +2848,10 @@
         <v>2.33999991</v>
       </c>
       <c r="D157">
-        <v>86.784741500965083</v>
+        <v>86.784741500965069</v>
       </c>
       <c r="E157">
-        <v>-5.1051863040331751e-14</v>
+        <v>-4.2632564145606011e-14</v>
       </c>
     </row>
     <row r="158">
@@ -2793,10 +2865,10 @@
         <v>2.27999997</v>
       </c>
       <c r="D158">
-        <v>83.643140118537374</v>
+        <v>83.64314011853736</v>
       </c>
       <c r="E158">
-        <v>8.5184202739047542e-14</v>
+        <v>5.6843418860808015e-14</v>
       </c>
     </row>
     <row r="159">
@@ -2813,7 +2885,7 @@
         <v>80.586063791498674</v>
       </c>
       <c r="E159">
-        <v>-6.1871852774186149e-14</v>
+        <v>-5.5067062021407764e-14</v>
       </c>
     </row>
     <row r="160">
@@ -2830,7 +2902,7 @@
         <v>77.619843078736963</v>
       </c>
       <c r="E160">
-        <v>3.0096396034238114e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -2844,10 +2916,10 @@
         <v>2.0999998999999998</v>
       </c>
       <c r="D161">
-        <v>74.747507218321047</v>
+        <v>74.74750721832109</v>
       </c>
       <c r="E161">
-        <v>-7.4778671645785699e-15</v>
+        <v>4.9737991503207013e-14</v>
       </c>
     </row>
     <row r="162">
@@ -2861,10 +2933,10 @@
         <v>2.0399999599999998</v>
       </c>
       <c r="D162">
-        <v>71.969940221323895</v>
+        <v>71.969940221323924</v>
       </c>
       <c r="E162">
-        <v>1.5053441319201797e-14</v>
+        <v>-5.3290705182007514e-15</v>
       </c>
     </row>
     <row r="163">
@@ -2878,10 +2950,10 @@
         <v>1.9800000200000001</v>
       </c>
       <c r="D163">
-        <v>69.286797706591884</v>
+        <v>69.286797706591912</v>
       </c>
       <c r="E163">
-        <v>5.4836874097107683e-15</v>
+        <v>5.3290705182007514e-15</v>
       </c>
     </row>
     <row r="164">
@@ -2895,10 +2967,10 @@
         <v>1.9199999599999999</v>
       </c>
       <c r="D164">
-        <v>66.697161580941611</v>
+        <v>66.697161580941639</v>
       </c>
       <c r="E164">
-        <v>-6.3404101984313185e-15</v>
+        <v>-2.3092638912203256e-14</v>
       </c>
     </row>
     <row r="165">
@@ -2912,10 +2984,10 @@
         <v>1.86000001</v>
       </c>
       <c r="D165">
-        <v>64.199982884110824</v>
+        <v>64.199982884110881</v>
       </c>
       <c r="E165">
-        <v>-5.2176997834986482e-14</v>
+        <v>-1.6875389974302379e-14</v>
       </c>
     </row>
     <row r="166">
@@ -2929,10 +3001,10 @@
         <v>1.7999999499999999</v>
       </c>
       <c r="D166">
-        <v>61.794372977262363</v>
+        <v>61.794372977262405</v>
       </c>
       <c r="E166">
-        <v>-1.0672461545026649e-14</v>
+        <v>-1.5099033134902129e-14</v>
       </c>
     </row>
     <row r="167">
@@ -2946,10 +3018,10 @@
         <v>1.7400000099999999</v>
       </c>
       <c r="D167">
-        <v>59.479789106099325</v>
+        <v>59.479789106099389</v>
       </c>
       <c r="E167">
-        <v>-2.1704069560538664e-14</v>
+        <v>-3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="168">
@@ -2963,10 +3035,10 @@
         <v>1.67999995</v>
       </c>
       <c r="D168">
-        <v>57.256160846152483</v>
+        <v>57.256160846152554</v>
       </c>
       <c r="E168">
-        <v>-3.1638731764282858e-14</v>
+        <v>-1.865174681370263e-14</v>
       </c>
     </row>
     <row r="169">
@@ -2980,10 +3052,10 @@
         <v>1.6200000000000001</v>
       </c>
       <c r="D169">
-        <v>55.123977079637349</v>
+        <v>55.12397707963742</v>
       </c>
       <c r="E169">
-        <v>3.0747881837513054e-14</v>
+        <v>1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="170">
@@ -2997,10 +3069,10 @@
         <v>1.55999994</v>
       </c>
       <c r="D170">
-        <v>53.084357352233674</v>
+        <v>53.084357352233759</v>
       </c>
       <c r="E170">
-        <v>-1.9123118949553568e-14</v>
+        <v>-1.3322676295501878e-14</v>
       </c>
     </row>
     <row r="171">
@@ -3014,10 +3086,10 @@
         <v>1.5</v>
       </c>
       <c r="D171">
-        <v>51.139100417991379</v>
+        <v>51.139100417991465</v>
       </c>
       <c r="E171">
-        <v>2.0398478113777159e-14</v>
+        <v>1.865174681370263e-14</v>
       </c>
     </row>
     <row r="172">
@@ -3031,10 +3103,10 @@
         <v>1.44000006</v>
       </c>
       <c r="D172">
-        <v>49.290688650588912</v>
+        <v>49.290688650589011</v>
       </c>
       <c r="E172">
-        <v>-1.4914123801674861e-14</v>
+        <v>-1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="173">
@@ -3048,10 +3120,10 @@
         <v>1.3799999999999999</v>
       </c>
       <c r="D173">
-        <v>47.542143228055515</v>
+        <v>47.542143228055608</v>
       </c>
       <c r="E173">
-        <v>1.304595264996115e-14</v>
+        <v>2.6645352591003757e-15</v>
       </c>
     </row>
     <row r="174">
@@ -3065,10 +3137,10 @@
         <v>1.32000005</v>
       </c>
       <c r="D174">
-        <v>45.896491983039176</v>
+        <v>45.896491983039276</v>
       </c>
       <c r="E174">
-        <v>1.2070491597163009e-14</v>
+        <v>7.9936057773011271e-15</v>
       </c>
     </row>
     <row r="175">
@@ -3082,10 +3154,10 @@
         <v>1.2599999900000001</v>
       </c>
       <c r="D175">
-        <v>44.355466518412804</v>
+        <v>44.355466518412911</v>
       </c>
       <c r="E175">
-        <v>1.3159040474843002e-14</v>
+        <v>2.1316282072803006e-14</v>
       </c>
     </row>
     <row r="176">
@@ -3099,10 +3171,10 @@
         <v>2.7300000199999999</v>
       </c>
       <c r="D176">
-        <v>86.579082707786554</v>
+        <v>86.57908270778654</v>
       </c>
       <c r="E176">
-        <v>4.7575773755715104e-14</v>
+        <v>2.8421709430404007e-14</v>
       </c>
     </row>
     <row r="177">
@@ -3116,10 +3188,10 @@
         <v>2.66000009</v>
       </c>
       <c r="D177">
-        <v>83.272578946613308</v>
+        <v>83.272578946613294</v>
       </c>
       <c r="E177">
-        <v>7.6152782074421214e-15</v>
+        <v>5.3290705182007514e-15</v>
       </c>
     </row>
     <row r="178">
@@ -3136,7 +3208,7 @@
         <v>80.089945841040588</v>
       </c>
       <c r="E178">
-        <v>6.4456626443253785e-14</v>
+        <v>6.3948846218409017e-14</v>
       </c>
     </row>
     <row r="179">
@@ -3150,10 +3222,10 @@
         <v>2.5199999800000001</v>
       </c>
       <c r="D179">
-        <v>77.032770120913838</v>
+        <v>77.032770120913852</v>
       </c>
       <c r="E179">
-        <v>1.2371582421833115e-15</v>
+        <v>2.4868995751603507e-14</v>
       </c>
     </row>
     <row r="180">
@@ -3170,7 +3242,7 @@
         <v>74.098239202991465</v>
       </c>
       <c r="E180">
-        <v>3.7828414292322301e-14</v>
+        <v>1.7763568394002505e-15</v>
       </c>
     </row>
     <row r="181">
@@ -3187,7 +3259,7 @@
         <v>71.281545417916661</v>
       </c>
       <c r="E181">
-        <v>3.2117700655247479e-14</v>
+        <v>8.8817841970012523e-15</v>
       </c>
     </row>
     <row r="182">
@@ -3201,10 +3273,10 @@
         <v>2.30999994</v>
       </c>
       <c r="D182">
-        <v>68.577338040019114</v>
+        <v>68.577338040019143</v>
       </c>
       <c r="E182">
-        <v>-9.3074310436070843e-15</v>
+        <v>1.7763568394002505e-15</v>
       </c>
     </row>
     <row r="183">
@@ -3218,10 +3290,10 @@
         <v>2.2400000100000002</v>
       </c>
       <c r="D183">
-        <v>65.980519235894846</v>
+        <v>65.980519235894889</v>
       </c>
       <c r="E183">
-        <v>-4.5904114595942172e-14</v>
+        <v>-1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="184">
@@ -3235,10 +3307,10 @@
         <v>2.1700000799999999</v>
       </c>
       <c r="D184">
-        <v>63.486652264406516</v>
+        <v>63.486652264406551</v>
       </c>
       <c r="E184">
-        <v>9.7777935168034504e-15</v>
+        <v>-1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="185">
@@ -3252,10 +3324,10 @@
         <v>2.0999998999999998</v>
       </c>
       <c r="D185">
-        <v>61.092147620068324</v>
+        <v>61.092147620068367</v>
       </c>
       <c r="E185">
-        <v>-9.8495308491635025e-15</v>
+        <v>-1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="186">
@@ -3269,10 +3341,10 @@
         <v>2.02999997</v>
       </c>
       <c r="D186">
-        <v>58.794338932277242</v>
+        <v>58.794338932277284</v>
       </c>
       <c r="E186">
-        <v>3.7655497042900342e-14</v>
+        <v>1.9539925233402755e-14</v>
       </c>
     </row>
     <row r="187">
@@ -3286,10 +3358,10 @@
         <v>1.9600000399999999</v>
       </c>
       <c r="D187">
-        <v>56.591518316362574</v>
+        <v>56.591518316362638</v>
       </c>
       <c r="E187">
-        <v>-2.3703202653752058e-14</v>
+        <v>-3.5527136788005009e-14</v>
       </c>
     </row>
     <row r="188">
@@ -3303,10 +3375,10 @@
         <v>1.88999999</v>
       </c>
       <c r="D188">
-        <v>54.48295711645968</v>
+        <v>54.482957116459772</v>
       </c>
       <c r="E188">
-        <v>-1.8368512341752172e-14</v>
+        <v>2.8421709430404007e-14</v>
       </c>
     </row>
     <row r="189">
@@ -3320,10 +3392,10 @@
         <v>1.82000005</v>
       </c>
       <c r="D189">
-        <v>52.468943873354156</v>
+        <v>52.468943873354242</v>
       </c>
       <c r="E189">
-        <v>1.2163650845533491e-14</v>
+        <v>1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="190">
@@ -3337,10 +3409,10 @@
         <v>1.75</v>
       </c>
       <c r="D190">
-        <v>50.550855244163316</v>
+        <v>50.550855244163394</v>
       </c>
       <c r="E190">
-        <v>-3.1962238639007636e-14</v>
+        <v>-5.2402526762307389e-14</v>
       </c>
     </row>
     <row r="191">
@@ -3354,10 +3426,10 @@
         <v>1.67999995</v>
       </c>
       <c r="D191">
-        <v>48.731250310875289</v>
+        <v>48.731250310875389</v>
       </c>
       <c r="E191">
-        <v>6.8945084413700293e-15</v>
+        <v>2.042810365310288e-14</v>
       </c>
     </row>
     <row r="192">
@@ -3371,10 +3443,10 @@
         <v>1.61000001</v>
       </c>
       <c r="D192">
-        <v>47.013927684192979</v>
+        <v>47.013927684193078</v>
       </c>
       <c r="E192">
-        <v>-1.1724665053512606e-14</v>
+        <v>-1.5987211554602254e-14</v>
       </c>
     </row>
     <row r="193">
@@ -3388,10 +3460,10 @@
         <v>1.5399999600000001</v>
       </c>
       <c r="D193">
-        <v>45.403640610537856</v>
+        <v>45.403640610537956</v>
       </c>
       <c r="E193">
-        <v>-1.5848394736286234e-14</v>
+        <v>-3.6415315207705135e-14</v>
       </c>
     </row>
     <row r="194">
@@ -3405,10 +3477,10 @@
         <v>1.47000003</v>
       </c>
       <c r="D194">
-        <v>43.90456861765572</v>
+        <v>43.904568617655833</v>
       </c>
       <c r="E194">
-        <v>-8.4074311229390425e-15</v>
+        <v>-3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="195">
@@ -3422,10 +3494,10 @@
         <v>3.1199998899999999</v>
       </c>
       <c r="D195">
-        <v>86.290910204280721</v>
+        <v>86.290910204280706</v>
       </c>
       <c r="E195">
-        <v>-2.3535878369566356e-14</v>
+        <v>-4.2632564145606011e-14</v>
       </c>
     </row>
     <row r="196">
@@ -3442,7 +3514,7 @@
         <v>82.769787279356294</v>
       </c>
       <c r="E196">
-        <v>2.9404691282973318e-14</v>
+        <v>3.1974423109204508e-14</v>
       </c>
     </row>
     <row r="197">
@@ -3456,10 +3528,10 @@
         <v>2.9600000400000002</v>
       </c>
       <c r="D197">
-        <v>79.436856314235541</v>
+        <v>79.436856314235555</v>
       </c>
       <c r="E197">
-        <v>-5.2015243499816382e-14</v>
+        <v>-4.0856207306205761e-14</v>
       </c>
     </row>
     <row r="198">
@@ -3473,10 +3545,10 @@
         <v>2.8800001100000001</v>
       </c>
       <c r="D198">
-        <v>76.280099756290184</v>
+        <v>76.280099756290198</v>
       </c>
       <c r="E198">
-        <v>-2.6838297784375215e-15</v>
+        <v>-1.7763568394002505e-15</v>
       </c>
     </row>
     <row r="199">
@@ -3490,10 +3562,10 @@
         <v>2.7999999500000001</v>
       </c>
       <c r="D199">
-        <v>73.284121619331387</v>
+        <v>73.284121619331401</v>
       </c>
       <c r="E199">
-        <v>3.0310275610976135e-15</v>
+        <v>2.3092638912203256e-14</v>
       </c>
     </row>
     <row r="200">
@@ -3507,10 +3579,10 @@
         <v>2.72000003</v>
       </c>
       <c r="D200">
-        <v>70.434032964041677</v>
+        <v>70.434032964041705</v>
       </c>
       <c r="E200">
-        <v>-6.1446155955921687e-14</v>
+        <v>-2.3092638912203256e-14</v>
       </c>
     </row>
     <row r="201">
@@ -3524,10 +3596,10 @@
         <v>2.6400001</v>
       </c>
       <c r="D201">
-        <v>67.71684409327618</v>
+        <v>67.716844093276208</v>
       </c>
       <c r="E201">
-        <v>3.272370999568818e-14</v>
+        <v>3.907985046680551e-14</v>
       </c>
     </row>
     <row r="202">
@@ -3541,10 +3613,10 @@
         <v>2.55999994</v>
       </c>
       <c r="D202">
-        <v>65.121777996136686</v>
+        <v>65.1217779961367</v>
       </c>
       <c r="E202">
-        <v>4.3484773190914765e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -3558,10 +3630,10 @@
         <v>2.4800000199999999</v>
       </c>
       <c r="D203">
-        <v>62.6401811548401</v>
+        <v>62.640181154840143</v>
       </c>
       <c r="E203">
-        <v>6.7675154356571361e-15</v>
+        <v>1.5987211554602254e-14</v>
       </c>
     </row>
     <row r="204">
@@ -3575,10 +3647,10 @@
         <v>2.4000001000000002</v>
       </c>
       <c r="D204">
-        <v>60.265323903883939</v>
+        <v>60.265323903883989</v>
       </c>
       <c r="E204">
-        <v>5.5824621211942518e-15</v>
+        <v>1.2434497875801753e-14</v>
       </c>
     </row>
     <row r="205">
@@ -3592,10 +3664,10 @@
         <v>2.3199999299999998</v>
       </c>
       <c r="D205">
-        <v>57.99219174365868</v>
+        <v>57.992191743658736</v>
       </c>
       <c r="E205">
-        <v>-6.3164339473099071e-15</v>
+        <v>-5.3290705182007514e-15</v>
       </c>
     </row>
     <row r="206">
@@ -3609,10 +3681,10 @@
         <v>2.2400000100000002</v>
       </c>
       <c r="D206">
-        <v>55.817317002117996</v>
+        <v>55.817317002118052</v>
       </c>
       <c r="E206">
-        <v>2.8627226722890507e-15</v>
+        <v>-3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="207">
@@ -3626,10 +3698,10 @@
         <v>2.16000009</v>
       </c>
       <c r="D207">
-        <v>53.738675961592996</v>
+        <v>53.73867596159306</v>
       </c>
       <c r="E207">
-        <v>1.2943704071559569e-14</v>
+        <v>-1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="208">
@@ -3643,10 +3715,10 @@
         <v>2.0799999200000001</v>
       </c>
       <c r="D208">
-        <v>51.755651896681471</v>
+        <v>51.755651896681556</v>
       </c>
       <c r="E208">
-        <v>-3.072594548651578e-14</v>
+        <v>-7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="209">
@@ -3660,10 +3732,10 @@
         <v>2</v>
       </c>
       <c r="D209">
-        <v>49.869091171963696</v>
+        <v>49.869091171963781</v>
       </c>
       <c r="E209">
-        <v>4.8394741610432147e-15</v>
+        <v>-1.7763568394002505e-15</v>
       </c>
     </row>
     <row r="210">
@@ -3677,10 +3749,10 @@
         <v>1.9199999599999999</v>
       </c>
       <c r="D210">
-        <v>48.081493946243064</v>
+        <v>48.081493946243164</v>
       </c>
       <c r="E210">
-        <v>3.0198845616367746e-14</v>
+        <v>5.0626169922907138e-14</v>
       </c>
     </row>
     <row r="211">
@@ -3694,10 +3766,10 @@
         <v>1.8400000299999999</v>
       </c>
       <c r="D211">
-        <v>46.397366289467755</v>
+        <v>46.397366289467861</v>
       </c>
       <c r="E211">
-        <v>-1.5670564455552295e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -3711,10 +3783,10 @@
         <v>1.7599999900000001</v>
       </c>
       <c r="D212">
-        <v>44.823677313797596</v>
+        <v>44.82367731379771</v>
       </c>
       <c r="E212">
-        <v>5.6072706210490935e-16</v>
+        <v>1.7763568394002505e-15</v>
       </c>
     </row>
     <row r="213">
@@ -3728,10 +3800,10 @@
         <v>1.67999995</v>
       </c>
       <c r="D213">
-        <v>43.369340330028741</v>
+        <v>43.369340330028876</v>
       </c>
       <c r="E213">
-        <v>-7.22565158156031e-15</v>
+        <v>3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="214">
@@ -3745,10 +3817,10 @@
         <v>3.5099999899999998</v>
       </c>
       <c r="D214">
-        <v>85.852401208943462</v>
+        <v>85.852401208943448</v>
       </c>
       <c r="E214">
-        <v>5.6088808971247078e-14</v>
+        <v>1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="215">
@@ -3765,7 +3837,7 @@
         <v>82.053338211079819</v>
       </c>
       <c r="E215">
-        <v>-1.783436785204549e-14</v>
+        <v>-2.1316282072803006e-14</v>
       </c>
     </row>
     <row r="216">
@@ -3779,10 +3851,10 @@
         <v>3.3299999200000001</v>
       </c>
       <c r="D216">
-        <v>78.554734703964797</v>
+        <v>78.554734703964812</v>
       </c>
       <c r="E216">
-        <v>-6.3755342884396092e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -3796,10 +3868,10 @@
         <v>3.2400000100000002</v>
       </c>
       <c r="D217">
-        <v>75.304892012306993</v>
+        <v>75.304892012307022</v>
       </c>
       <c r="E217">
-        <v>1.2260308440788196e-14</v>
+        <v>4.9737991503207013e-14</v>
       </c>
     </row>
     <row r="218">
@@ -3813,10 +3885,10 @@
         <v>3.1500001000000002</v>
       </c>
       <c r="D218">
-        <v>72.262447891954764</v>
+        <v>72.262447891954778</v>
       </c>
       <c r="E218">
-        <v>-6.6795156966413443e-16</v>
+        <v>-2.8421709430404007e-14</v>
       </c>
     </row>
     <row r="219">
@@ -3830,10 +3902,10 @@
         <v>3.05999994</v>
       </c>
       <c r="D219">
-        <v>69.396260768195361</v>
+        <v>69.39626076819539</v>
       </c>
       <c r="E219">
-        <v>-1.5018153360239334e-14</v>
+        <v>3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="220">
@@ -3847,10 +3919,10 @@
         <v>2.97000003</v>
       </c>
       <c r="D220">
-        <v>66.683051005245247</v>
+        <v>66.683051005245275</v>
       </c>
       <c r="E220">
-        <v>2.3811863562949741e-14</v>
+        <v>3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="221">
@@ -3864,10 +3936,10 @@
         <v>2.8800001100000001</v>
       </c>
       <c r="D221">
-        <v>64.105332737752022</v>
+        <v>64.105332737752065</v>
       </c>
       <c r="E221">
-        <v>-1.1333434539613727e-14</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="222">
@@ -3881,10 +3953,10 @@
         <v>2.7899999599999998</v>
       </c>
       <c r="D222">
-        <v>61.649928409171871</v>
+        <v>61.64992840917192</v>
       </c>
       <c r="E222">
-        <v>-5.9032670537838336e-15</v>
+        <v>1.0658141036401503e-14</v>
       </c>
     </row>
     <row r="223">
@@ -3898,10 +3970,10 @@
         <v>2.7000000499999999</v>
       </c>
       <c r="D223">
-        <v>59.306956101486435</v>
+        <v>59.306956101486499</v>
       </c>
       <c r="E223">
-        <v>-5.8296446131759017e-14</v>
+        <v>-3.907985046680551e-14</v>
       </c>
     </row>
     <row r="224">
@@ -3915,10 +3987,10 @@
         <v>2.6099999</v>
       </c>
       <c r="D224">
-        <v>57.06915295913339</v>
+        <v>57.069152959133454</v>
       </c>
       <c r="E224">
-        <v>-3.2988940907261229e-14</v>
+        <v>-1.4210854715202004e-14</v>
       </c>
     </row>
     <row r="225">
@@ -3932,10 +4004,10 @@
         <v>2.5199999800000001</v>
       </c>
       <c r="D225">
-        <v>54.931414687579533</v>
+        <v>54.931414687579597</v>
       </c>
       <c r="E225">
-        <v>1.3174297401976127e-15</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="226">
@@ -3949,10 +4021,10 @@
         <v>2.4300000700000002</v>
       </c>
       <c r="D226">
-        <v>52.890516525865124</v>
+        <v>52.890516525865188</v>
       </c>
       <c r="E226">
-        <v>9.5365767163026474e-15</v>
+        <v>3.5527136788005009e-15</v>
       </c>
     </row>
     <row r="227">
@@ -3966,10 +4038,10 @@
         <v>2.33999991</v>
       </c>
       <c r="D227">
-        <v>50.944968172435281</v>
+        <v>50.944968172435352</v>
       </c>
       <c r="E227">
-        <v>3.250230232591603e-14</v>
+        <v>3.1974423109204508e-14</v>
       </c>
     </row>
     <row r="228">
@@ -3983,10 +4055,10 @@
         <v>2.25</v>
       </c>
       <c r="D228">
-        <v>49.09501709773793</v>
+        <v>49.095017097738008</v>
       </c>
       <c r="E228">
-        <v>-8.4343343213315569e-15</v>
+        <v>-1.7763568394002505e-14</v>
       </c>
     </row>
     <row r="229">
@@ -4000,10 +4072,10 @@
         <v>2.16000009</v>
       </c>
       <c r="D229">
-        <v>47.342859149478919</v>
+        <v>47.342859149479011</v>
       </c>
       <c r="E229">
-        <v>2.3627965548466702e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230">
@@ -4017,10 +4089,10 @@
         <v>2.0699999299999998</v>
       </c>
       <c r="D230">
-        <v>45.693185533746451</v>
+        <v>45.693185533746558</v>
       </c>
       <c r="E230">
-        <v>1.0001023093717847e-14</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="231">
@@ -4034,10 +4106,10 @@
         <v>1.9800000200000001</v>
       </c>
       <c r="D231">
-        <v>44.154440987663769</v>
+        <v>44.154440987663889</v>
       </c>
       <c r="E231">
-        <v>-8.9768701565796145e-15</v>
+        <v>7.1054273576010019e-15</v>
       </c>
     </row>
     <row r="232">
@@ -4051,10 +4123,10 @@
         <v>1.88999999</v>
       </c>
       <c r="D232">
-        <v>42.741506553010467</v>
+        <v>42.741506553010609</v>
       </c>
       <c r="E232">
-        <v>-2.168870414878135e-14</v>
+        <v>1.4210854715202004e-14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>